<commit_message>
add synthetic data set simple vs real
</commit_message>
<xml_diff>
--- a/tasks/mcra/examples/task_input/test_mcra_action_template/Data/Compounds.xlsx
+++ b/tasks/mcra/examples/task_input/test_mcra_action_template/Data/Compounds.xlsx
@@ -599,41 +599,41 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>CPF</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TestCompoundA</t>
+          <t>Chlorpyrifos</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Synthetic test compound</t>
+          <t>Organophosphate insecticide (synthetic test data)</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.01</v>
+        <v>0.005</v>
       </c>
       <c r="E2" t="n">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>mg/kg</t>
+          <t>mgPerKg</t>
         </is>
       </c>
       <c r="H2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>350.6</v>
+      </c>
+      <c r="J2" t="b">
         <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>250</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>